<commit_message>
more updates to documentation and also updated vehicle (Diego)
</commit_message>
<xml_diff>
--- a/documentation/trials.xlsx
+++ b/documentation/trials.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ocean\Documents\GitHub\CPTS-437-DDPG-RSSI-Car\documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2B25D297-6076-4EAC-A047-E9AA9AEAA332}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9DB5B4EC-263F-4C4E-9F91-12741190E2DB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{496E26A4-E262-4A0D-A9DD-90AD4307AC27}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="22">
   <si>
     <t>memory_size</t>
   </si>
@@ -84,6 +84,24 @@
   </si>
   <si>
     <t>MAX_SENSOR_MEASUREMENT</t>
+  </si>
+  <si>
+    <t>Bad</t>
+  </si>
+  <si>
+    <t>Comments</t>
+  </si>
+  <si>
+    <t>Very Bad</t>
+  </si>
+  <si>
+    <t>Ok</t>
+  </si>
+  <si>
+    <t>Meh</t>
+  </si>
+  <si>
+    <t>Simulation</t>
   </si>
 </sst>
 </file>
@@ -458,10 +476,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DD51C088-492E-456A-BAA7-804EE5452A68}">
-  <dimension ref="A1:L8"/>
+  <dimension ref="A1:N8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="N15" sqref="N15"/>
+      <selection sqref="A1:N8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -474,311 +492,358 @@
     <col min="7" max="7" width="12" style="1" bestFit="1" customWidth="1"/>
     <col min="8" max="9" width="14.6640625" style="1" bestFit="1" customWidth="1"/>
     <col min="10" max="11" width="14.5546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="12" max="16384" width="8.88671875" style="1"/>
+    <col min="12" max="12" width="8.88671875" style="1"/>
+    <col min="13" max="13" width="9.77734375" style="1" bestFit="1" customWidth="1"/>
+    <col min="14" max="16384" width="8.88671875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>7</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>1</v>
+        <v>21</v>
       </c>
       <c r="C1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="I1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="J1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="K1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="L1" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="L1" s="1" t="s">
+      <c r="M1" s="1" t="s">
         <v>9</v>
       </c>
+      <c r="N1" s="1" t="s">
+        <v>17</v>
+      </c>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A2" s="1">
         <v>1</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="B2" s="1">
+        <v>1</v>
+      </c>
+      <c r="C2" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="C2" s="1">
-        <v>1</v>
-      </c>
       <c r="D2" s="1">
+        <v>1</v>
+      </c>
+      <c r="E2" s="1">
         <v>0.5</v>
       </c>
-      <c r="E2" s="1">
+      <c r="F2" s="1">
         <v>10</v>
       </c>
-      <c r="F2" s="1">
+      <c r="G2" s="1">
         <v>128</v>
       </c>
-      <c r="G2" s="1">
+      <c r="H2" s="1">
         <v>3</v>
       </c>
-      <c r="H2" s="1">
+      <c r="I2" s="1">
         <v>0.99</v>
       </c>
-      <c r="I2" s="1">
+      <c r="J2" s="1">
         <v>4000</v>
       </c>
-      <c r="J2" s="1">
+      <c r="K2" s="1">
         <v>1000</v>
       </c>
-      <c r="K2" s="1">
-        <v>1</v>
-      </c>
-      <c r="L2" s="1" t="s">
+      <c r="L2" s="1">
+        <v>1</v>
+      </c>
+      <c r="M2" s="1" t="s">
         <v>10</v>
       </c>
+      <c r="N2" s="1" t="s">
+        <v>16</v>
+      </c>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A3" s="1">
         <v>2</v>
       </c>
-      <c r="B3" s="1" t="s">
+      <c r="B3" s="1">
+        <v>1</v>
+      </c>
+      <c r="C3" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="C3" s="1">
+      <c r="D3" s="1">
         <v>4</v>
       </c>
-      <c r="D3" s="1">
+      <c r="E3" s="1">
         <v>0.5</v>
       </c>
-      <c r="E3" s="1">
+      <c r="F3" s="1">
         <v>10</v>
       </c>
-      <c r="F3" s="1">
+      <c r="G3" s="1">
         <v>128</v>
       </c>
-      <c r="G3" s="1">
+      <c r="H3" s="1">
         <v>3</v>
       </c>
-      <c r="H3" s="1">
+      <c r="I3" s="1">
         <v>0.99</v>
       </c>
-      <c r="I3" s="1">
+      <c r="J3" s="1">
         <v>4000</v>
       </c>
-      <c r="J3" s="1">
+      <c r="K3" s="1">
         <v>1000</v>
       </c>
-      <c r="K3" s="1">
-        <v>1</v>
-      </c>
-      <c r="L3" s="1" t="s">
-        <v>11</v>
+      <c r="L3" s="1">
+        <v>1</v>
+      </c>
+      <c r="M3" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="N3" s="1" t="s">
+        <v>16</v>
       </c>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A4" s="1">
         <v>3</v>
       </c>
-      <c r="B4" s="1" t="s">
+      <c r="B4" s="1">
+        <v>1</v>
+      </c>
+      <c r="C4" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="C4" s="1">
+      <c r="D4" s="1">
         <v>4</v>
       </c>
-      <c r="D4" s="1">
+      <c r="E4" s="1">
         <v>0.5</v>
       </c>
-      <c r="E4" s="1">
+      <c r="F4" s="1">
         <v>5</v>
       </c>
-      <c r="F4" s="1">
+      <c r="G4" s="1">
         <v>128</v>
       </c>
-      <c r="G4" s="1">
+      <c r="H4" s="1">
         <v>3</v>
       </c>
-      <c r="H4" s="1">
+      <c r="I4" s="1">
         <v>0.99</v>
       </c>
-      <c r="I4" s="1">
+      <c r="J4" s="1">
         <v>4000</v>
       </c>
-      <c r="J4" s="1">
+      <c r="K4" s="1">
         <v>1000</v>
       </c>
-      <c r="K4" s="1">
-        <v>1</v>
-      </c>
-      <c r="L4" s="1" t="s">
+      <c r="L4" s="1">
+        <v>1</v>
+      </c>
+      <c r="M4" s="1" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A5" s="1">
         <v>4</v>
       </c>
-      <c r="B5" s="1" t="s">
+      <c r="B5" s="1">
+        <v>1</v>
+      </c>
+      <c r="C5" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="C5" s="1">
+      <c r="D5" s="1">
         <v>4</v>
       </c>
-      <c r="D5" s="1">
+      <c r="E5" s="1">
         <v>0.5</v>
       </c>
-      <c r="E5" s="1">
-        <v>1</v>
-      </c>
       <c r="F5" s="1">
+        <v>1</v>
+      </c>
+      <c r="G5" s="1">
         <v>128</v>
       </c>
-      <c r="G5" s="1">
+      <c r="H5" s="1">
         <v>3</v>
       </c>
-      <c r="H5" s="1">
+      <c r="I5" s="1">
         <v>0.99</v>
       </c>
-      <c r="I5" s="1">
+      <c r="J5" s="1">
         <v>4000</v>
       </c>
-      <c r="J5" s="1">
+      <c r="K5" s="1">
         <v>1000</v>
       </c>
-      <c r="K5" s="1">
-        <v>1</v>
-      </c>
-      <c r="L5" s="1" t="s">
+      <c r="L5" s="1">
+        <v>1</v>
+      </c>
+      <c r="M5" s="1" t="s">
         <v>11</v>
       </c>
+      <c r="N5" s="1" t="s">
+        <v>18</v>
+      </c>
     </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A6" s="1">
         <v>5</v>
       </c>
-      <c r="B6" s="1" t="s">
+      <c r="B6" s="1">
+        <v>1</v>
+      </c>
+      <c r="C6" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="C6" s="1">
+      <c r="D6" s="1">
         <v>4</v>
       </c>
-      <c r="D6" s="1">
+      <c r="E6" s="1">
         <v>0.5</v>
       </c>
-      <c r="E6" s="1">
+      <c r="F6" s="1">
         <v>5</v>
       </c>
-      <c r="F6" s="1">
+      <c r="G6" s="1">
         <v>64</v>
       </c>
-      <c r="G6" s="1">
+      <c r="H6" s="1">
         <v>2</v>
       </c>
-      <c r="H6" s="1">
+      <c r="I6" s="1">
         <v>0.99</v>
       </c>
-      <c r="I6" s="1">
+      <c r="J6" s="1">
         <v>4000</v>
       </c>
-      <c r="J6" s="1">
+      <c r="K6" s="1">
         <v>1000</v>
       </c>
-      <c r="K6" s="1">
-        <v>1</v>
-      </c>
-      <c r="L6" s="1" t="s">
-        <v>11</v>
+      <c r="L6" s="1">
+        <v>1</v>
+      </c>
+      <c r="M6" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="N6" s="1" t="s">
+        <v>19</v>
       </c>
     </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A7" s="1">
         <v>6</v>
       </c>
-      <c r="B7" s="1" t="s">
+      <c r="B7" s="1">
+        <v>1</v>
+      </c>
+      <c r="C7" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="C7" s="1">
+      <c r="D7" s="1">
         <v>4</v>
       </c>
-      <c r="D7" s="1">
+      <c r="E7" s="1">
         <v>0.5</v>
       </c>
-      <c r="E7" s="1">
+      <c r="F7" s="1">
         <v>5</v>
       </c>
-      <c r="F7" s="1">
+      <c r="G7" s="1">
         <v>64</v>
       </c>
-      <c r="G7" s="1">
+      <c r="H7" s="1">
         <v>2</v>
       </c>
-      <c r="H7" s="1">
+      <c r="I7" s="1">
         <v>0.95</v>
       </c>
-      <c r="I7" s="1">
+      <c r="J7" s="1">
         <v>4000</v>
       </c>
-      <c r="J7" s="1">
+      <c r="K7" s="1">
         <v>1000</v>
       </c>
-      <c r="K7" s="1">
-        <v>1</v>
-      </c>
-      <c r="L7" s="1" t="s">
+      <c r="L7" s="1">
+        <v>1</v>
+      </c>
+      <c r="M7" s="1" t="s">
         <v>11</v>
       </c>
+      <c r="N7" s="1" t="s">
+        <v>20</v>
+      </c>
     </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A8" s="1">
         <v>7</v>
       </c>
-      <c r="B8" s="1" t="s">
+      <c r="B8" s="1">
+        <v>1</v>
+      </c>
+      <c r="C8" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="C8" s="1">
+      <c r="D8" s="1">
         <v>4</v>
       </c>
-      <c r="D8" s="1">
+      <c r="E8" s="1">
         <v>0.5</v>
       </c>
-      <c r="E8" s="1">
+      <c r="F8" s="1">
         <v>5</v>
       </c>
-      <c r="F8" s="1">
+      <c r="G8" s="1">
         <v>64</v>
       </c>
-      <c r="G8" s="1">
+      <c r="H8" s="1">
         <v>2</v>
       </c>
-      <c r="H8" s="1">
+      <c r="I8" s="1">
         <v>0.9</v>
       </c>
-      <c r="I8" s="1">
+      <c r="J8" s="1">
         <v>4000</v>
       </c>
-      <c r="J8" s="1">
+      <c r="K8" s="1">
         <v>1000</v>
       </c>
-      <c r="K8" s="1">
-        <v>1</v>
-      </c>
-      <c r="L8" s="1" t="s">
+      <c r="L8" s="1">
+        <v>1</v>
+      </c>
+      <c r="M8" s="1" t="s">
         <v>11</v>
+      </c>
+      <c r="N8" s="1" t="s">
+        <v>16</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updated README, documentation. Major changes to config and simulation
</commit_message>
<xml_diff>
--- a/documentation/trials.xlsx
+++ b/documentation/trials.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ocean\Documents\GitHub\CPTS-437-DDPG-RSSI-Car\documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9DB5B4EC-263F-4C4E-9F91-12741190E2DB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E08FE1A8-E4CD-48F3-9B01-2FEFC55A6540}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{496E26A4-E262-4A0D-A9DD-90AD4307AC27}"/>
   </bookViews>
@@ -36,14 +36,11 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="22">
   <si>
     <t>memory_size</t>
   </si>
   <si>
-    <t>Obstacles</t>
-  </si>
-  <si>
     <t>hidden_neurons</t>
   </si>
   <si>
@@ -102,6 +99,9 @@
   </si>
   <si>
     <t>Simulation</t>
+  </si>
+  <si>
+    <t>obstacle_types</t>
   </si>
 </sst>
 </file>
@@ -476,69 +476,66 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DD51C088-492E-456A-BAA7-804EE5452A68}">
-  <dimension ref="A1:N8"/>
+  <dimension ref="A1:N9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:N8"/>
+      <selection activeCell="E17" sqref="E17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="8.33203125" style="1" customWidth="1"/>
-    <col min="2" max="2" width="14.6640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.6640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="25.88671875" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="6" width="13.88671875" style="1" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="12" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="14.6640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="5" width="25.88671875" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="7" width="13.88671875" style="1" bestFit="1" customWidth="1"/>
     <col min="8" max="9" width="14.6640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="10" max="11" width="14.5546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="8.88671875" style="1"/>
-    <col min="13" max="13" width="9.77734375" style="1" bestFit="1" customWidth="1"/>
-    <col min="14" max="16384" width="8.88671875" style="1"/>
+    <col min="10" max="12" width="14.5546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="13" max="14" width="9.77734375" style="1" bestFit="1" customWidth="1"/>
+    <col min="15" max="16384" width="8.88671875" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="D1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="B1" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>8</v>
-      </c>
       <c r="E1" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="F1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="G1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="H1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="I1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="J1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="K1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="K1" s="1" t="s">
-        <v>6</v>
-      </c>
       <c r="L1" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="M1" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="N1" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="2" spans="1:14" x14ac:dyDescent="0.3">
@@ -549,7 +546,7 @@
         <v>1</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D2" s="1">
         <v>1</v>
@@ -579,10 +576,10 @@
         <v>1</v>
       </c>
       <c r="M2" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="N2" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="3" spans="1:14" x14ac:dyDescent="0.3">
@@ -593,7 +590,7 @@
         <v>1</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D3" s="1">
         <v>4</v>
@@ -623,10 +620,10 @@
         <v>1</v>
       </c>
       <c r="M3" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="N3" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="4" spans="1:14" x14ac:dyDescent="0.3">
@@ -637,7 +634,7 @@
         <v>1</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D4" s="1">
         <v>4</v>
@@ -667,7 +664,7 @@
         <v>1</v>
       </c>
       <c r="M4" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="5" spans="1:14" x14ac:dyDescent="0.3">
@@ -678,7 +675,7 @@
         <v>1</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D5" s="1">
         <v>4</v>
@@ -708,10 +705,10 @@
         <v>1</v>
       </c>
       <c r="M5" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="N5" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="6" spans="1:14" x14ac:dyDescent="0.3">
@@ -722,7 +719,7 @@
         <v>1</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D6" s="1">
         <v>4</v>
@@ -752,10 +749,10 @@
         <v>1</v>
       </c>
       <c r="M6" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="N6" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="7" spans="1:14" x14ac:dyDescent="0.3">
@@ -766,7 +763,7 @@
         <v>1</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D7" s="1">
         <v>4</v>
@@ -796,10 +793,10 @@
         <v>1</v>
       </c>
       <c r="M7" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="N7" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="8" spans="1:14" x14ac:dyDescent="0.3">
@@ -810,7 +807,7 @@
         <v>1</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D8" s="1">
         <v>4</v>
@@ -840,10 +837,51 @@
         <v>1</v>
       </c>
       <c r="M8" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="N8" s="1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="9" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A9" s="1">
+        <v>8</v>
+      </c>
+      <c r="B9" s="1">
+        <v>2</v>
+      </c>
+      <c r="C9" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="N8" s="1" t="s">
-        <v>16</v>
+      <c r="D9" s="1">
+        <v>4</v>
+      </c>
+      <c r="E9" s="1">
+        <v>0.5</v>
+      </c>
+      <c r="F9" s="1">
+        <v>5</v>
+      </c>
+      <c r="G9" s="1">
+        <v>64</v>
+      </c>
+      <c r="H9" s="1">
+        <v>2</v>
+      </c>
+      <c r="I9" s="1">
+        <v>0.99</v>
+      </c>
+      <c r="J9" s="1">
+        <v>4000</v>
+      </c>
+      <c r="K9" s="1">
+        <v>1000</v>
+      </c>
+      <c r="L9" s="1">
+        <v>2</v>
+      </c>
+      <c r="M9" s="1" t="s">
+        <v>10</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added trials 10-15 and documentation
</commit_message>
<xml_diff>
--- a/documentation/trials.xlsx
+++ b/documentation/trials.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ocean\Documents\GitHub\CPTS-437-DDPG-RSSI-Car\documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{29A4A610-98AF-4BA8-94A0-C7F0DB601E8C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{34E2F94F-A29A-45A2-8211-0B8EE7D3A184}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{496E26A4-E262-4A0D-A9DD-90AD4307AC27}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="29">
   <si>
     <t>memory_size</t>
   </si>
@@ -89,9 +89,6 @@
     <t>Comments</t>
   </si>
   <si>
-    <t>Very Bad</t>
-  </si>
-  <si>
     <t>Ok</t>
   </si>
   <si>
@@ -108,6 +105,24 @@
   </si>
   <si>
     <t>Hallway (random)</t>
+  </si>
+  <si>
+    <t>gae-lambda</t>
+  </si>
+  <si>
+    <t>Hallway (setups)</t>
+  </si>
+  <si>
+    <t>Train more</t>
+  </si>
+  <si>
+    <t>Very bad</t>
+  </si>
+  <si>
+    <t>clip_ratio</t>
+  </si>
+  <si>
+    <t>target_kl</t>
   </si>
 </sst>
 </file>
@@ -482,10 +497,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DD51C088-492E-456A-BAA7-804EE5452A68}">
-  <dimension ref="A1:N11"/>
+  <dimension ref="A1:Q19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C14" sqref="C14"/>
+      <selection activeCell="Q20" sqref="Q20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -495,21 +510,24 @@
     <col min="3" max="3" width="15.109375" style="1" bestFit="1" customWidth="1"/>
     <col min="4" max="5" width="25.88671875" style="1" bestFit="1" customWidth="1"/>
     <col min="6" max="7" width="13.88671875" style="1" bestFit="1" customWidth="1"/>
-    <col min="8" max="9" width="14.6640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="10" max="12" width="14.5546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="13" max="14" width="9.77734375" style="1" bestFit="1" customWidth="1"/>
-    <col min="15" max="16384" width="8.88671875" style="1"/>
+    <col min="8" max="8" width="14.6640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="9" max="10" width="14.6640625" style="1" customWidth="1"/>
+    <col min="11" max="11" width="14.6640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="12" max="15" width="14.5546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="9.77734375" style="1" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="15.88671875" style="1" bestFit="1" customWidth="1"/>
+    <col min="18" max="16384" width="8.88671875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>6</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>20</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>21</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>7</v>
@@ -527,25 +545,34 @@
         <v>2</v>
       </c>
       <c r="I1" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="K1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="J1" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="K1" s="1" t="s">
-        <v>5</v>
-      </c>
       <c r="L1" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="N1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="O1" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="M1" s="1" t="s">
+      <c r="P1" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="N1" s="1" t="s">
+      <c r="Q1" s="1" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A2" s="1">
         <v>1</v>
       </c>
@@ -571,25 +598,34 @@
         <v>3</v>
       </c>
       <c r="I2" s="1">
+        <v>0.2</v>
+      </c>
+      <c r="J2" s="1">
+        <v>0.01</v>
+      </c>
+      <c r="K2" s="1">
         <v>0.99</v>
       </c>
-      <c r="J2" s="1">
-        <v>4000</v>
-      </c>
-      <c r="K2" s="1">
+      <c r="L2" s="1">
+        <v>0.95</v>
+      </c>
+      <c r="M2" s="1">
+        <v>4000</v>
+      </c>
+      <c r="N2" s="1">
         <v>1000</v>
       </c>
-      <c r="L2" s="1">
-        <v>1</v>
-      </c>
-      <c r="M2" s="1" t="s">
+      <c r="O2" s="1">
+        <v>1</v>
+      </c>
+      <c r="P2" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="N2" s="1" t="s">
+      <c r="Q2" s="1" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A3" s="1">
         <v>2</v>
       </c>
@@ -615,25 +651,34 @@
         <v>3</v>
       </c>
       <c r="I3" s="1">
+        <v>0.2</v>
+      </c>
+      <c r="J3" s="1">
+        <v>0.01</v>
+      </c>
+      <c r="K3" s="1">
         <v>0.99</v>
       </c>
-      <c r="J3" s="1">
-        <v>4000</v>
-      </c>
-      <c r="K3" s="1">
+      <c r="L3" s="1">
+        <v>0.95</v>
+      </c>
+      <c r="M3" s="1">
+        <v>4000</v>
+      </c>
+      <c r="N3" s="1">
         <v>1000</v>
       </c>
-      <c r="L3" s="1">
-        <v>1</v>
-      </c>
-      <c r="M3" s="1" t="s">
+      <c r="O3" s="1">
+        <v>1</v>
+      </c>
+      <c r="P3" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="N3" s="1" t="s">
+      <c r="Q3" s="1" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A4" s="1">
         <v>3</v>
       </c>
@@ -659,22 +704,31 @@
         <v>3</v>
       </c>
       <c r="I4" s="1">
+        <v>0.2</v>
+      </c>
+      <c r="J4" s="1">
+        <v>0.01</v>
+      </c>
+      <c r="K4" s="1">
         <v>0.99</v>
       </c>
-      <c r="J4" s="1">
-        <v>4000</v>
-      </c>
-      <c r="K4" s="1">
+      <c r="L4" s="1">
+        <v>0.95</v>
+      </c>
+      <c r="M4" s="1">
+        <v>4000</v>
+      </c>
+      <c r="N4" s="1">
         <v>1000</v>
       </c>
-      <c r="L4" s="1">
-        <v>1</v>
-      </c>
-      <c r="M4" s="1" t="s">
+      <c r="O4" s="1">
+        <v>1</v>
+      </c>
+      <c r="P4" s="1" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A5" s="1">
         <v>4</v>
       </c>
@@ -700,25 +754,34 @@
         <v>3</v>
       </c>
       <c r="I5" s="1">
+        <v>0.2</v>
+      </c>
+      <c r="J5" s="1">
+        <v>0.01</v>
+      </c>
+      <c r="K5" s="1">
         <v>0.99</v>
       </c>
-      <c r="J5" s="1">
-        <v>4000</v>
-      </c>
-      <c r="K5" s="1">
+      <c r="L5" s="1">
+        <v>0.95</v>
+      </c>
+      <c r="M5" s="1">
+        <v>4000</v>
+      </c>
+      <c r="N5" s="1">
         <v>1000</v>
       </c>
-      <c r="L5" s="1">
-        <v>1</v>
-      </c>
-      <c r="M5" s="1" t="s">
+      <c r="O5" s="1">
+        <v>1</v>
+      </c>
+      <c r="P5" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="N5" s="1" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="Q5" s="1" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="6" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A6" s="1">
         <v>5</v>
       </c>
@@ -744,25 +807,34 @@
         <v>2</v>
       </c>
       <c r="I6" s="1">
+        <v>0.2</v>
+      </c>
+      <c r="J6" s="1">
+        <v>0.01</v>
+      </c>
+      <c r="K6" s="1">
         <v>0.99</v>
       </c>
-      <c r="J6" s="1">
-        <v>4000</v>
-      </c>
-      <c r="K6" s="1">
+      <c r="L6" s="1">
+        <v>0.95</v>
+      </c>
+      <c r="M6" s="1">
+        <v>4000</v>
+      </c>
+      <c r="N6" s="1">
         <v>1000</v>
       </c>
-      <c r="L6" s="1">
-        <v>1</v>
-      </c>
-      <c r="M6" s="1" t="s">
+      <c r="O6" s="1">
+        <v>1</v>
+      </c>
+      <c r="P6" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="N6" s="1" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="Q6" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="7" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A7" s="1">
         <v>6</v>
       </c>
@@ -788,25 +860,34 @@
         <v>2</v>
       </c>
       <c r="I7" s="1">
-        <v>0.95</v>
+        <v>0.2</v>
       </c>
       <c r="J7" s="1">
-        <v>4000</v>
+        <v>0.01</v>
       </c>
       <c r="K7" s="1">
+        <v>0.95</v>
+      </c>
+      <c r="L7" s="1">
+        <v>0.95</v>
+      </c>
+      <c r="M7" s="1">
+        <v>4000</v>
+      </c>
+      <c r="N7" s="1">
         <v>1000</v>
       </c>
-      <c r="L7" s="1">
-        <v>1</v>
-      </c>
-      <c r="M7" s="1" t="s">
+      <c r="O7" s="1">
+        <v>1</v>
+      </c>
+      <c r="P7" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="N7" s="1" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="Q7" s="1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="8" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A8" s="1">
         <v>7</v>
       </c>
@@ -832,25 +913,34 @@
         <v>2</v>
       </c>
       <c r="I8" s="1">
+        <v>0.2</v>
+      </c>
+      <c r="J8" s="1">
+        <v>0.01</v>
+      </c>
+      <c r="K8" s="1">
         <v>0.9</v>
       </c>
-      <c r="J8" s="1">
-        <v>4000</v>
-      </c>
-      <c r="K8" s="1">
+      <c r="L8" s="1">
+        <v>0.95</v>
+      </c>
+      <c r="M8" s="1">
+        <v>4000</v>
+      </c>
+      <c r="N8" s="1">
         <v>1000</v>
       </c>
-      <c r="L8" s="1">
-        <v>1</v>
-      </c>
-      <c r="M8" s="1" t="s">
+      <c r="O8" s="1">
+        <v>1</v>
+      </c>
+      <c r="P8" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="N8" s="1" t="s">
+      <c r="Q8" s="1" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A9" s="1">
         <v>8</v>
       </c>
@@ -876,25 +966,34 @@
         <v>2</v>
       </c>
       <c r="I9" s="1">
+        <v>0.2</v>
+      </c>
+      <c r="J9" s="1">
+        <v>0.01</v>
+      </c>
+      <c r="K9" s="1">
         <v>0.99</v>
       </c>
-      <c r="J9" s="1">
-        <v>4000</v>
-      </c>
-      <c r="K9" s="1">
+      <c r="L9" s="1">
+        <v>0.95</v>
+      </c>
+      <c r="M9" s="1">
+        <v>4000</v>
+      </c>
+      <c r="N9" s="1">
         <v>200</v>
       </c>
-      <c r="L9" s="1">
-        <v>2</v>
-      </c>
-      <c r="M9" s="1" t="s">
+      <c r="O9" s="1">
+        <v>2</v>
+      </c>
+      <c r="P9" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="N9" s="1" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="Q9" s="1" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="10" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A10" s="1">
         <v>8</v>
       </c>
@@ -902,7 +1001,7 @@
         <v>2</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D10" s="1">
         <v>4</v>
@@ -920,25 +1019,34 @@
         <v>2</v>
       </c>
       <c r="I10" s="1">
+        <v>0.2</v>
+      </c>
+      <c r="J10" s="1">
+        <v>0.01</v>
+      </c>
+      <c r="K10" s="1">
         <v>0.99</v>
       </c>
-      <c r="J10" s="1">
-        <v>4000</v>
-      </c>
-      <c r="K10" s="1">
+      <c r="L10" s="1">
+        <v>0.95</v>
+      </c>
+      <c r="M10" s="1">
+        <v>4000</v>
+      </c>
+      <c r="N10" s="1">
         <v>200</v>
       </c>
-      <c r="L10" s="1">
-        <v>2</v>
-      </c>
-      <c r="M10" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="N10" s="1" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="O10" s="1">
+        <v>2</v>
+      </c>
+      <c r="P10" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="Q10" s="1" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="11" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A11" s="1">
         <v>9</v>
       </c>
@@ -946,7 +1054,7 @@
         <v>2</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D11" s="1">
         <v>4</v>
@@ -964,16 +1072,455 @@
         <v>2</v>
       </c>
       <c r="I11" s="1">
+        <v>0.2</v>
+      </c>
+      <c r="J11" s="1">
+        <v>0.01</v>
+      </c>
+      <c r="K11" s="1">
         <v>0.99</v>
       </c>
-      <c r="J11" s="1">
-        <v>4000</v>
-      </c>
-      <c r="K11" s="1">
+      <c r="L11" s="1">
+        <v>0.95</v>
+      </c>
+      <c r="M11" s="1">
+        <v>4000</v>
+      </c>
+      <c r="N11" s="1">
         <v>200</v>
       </c>
-      <c r="L11" s="1">
-        <v>2</v>
+      <c r="O11" s="1">
+        <v>2</v>
+      </c>
+      <c r="P11" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="Q11" s="1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="12" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A12" s="1">
+        <v>10</v>
+      </c>
+      <c r="B12" s="1">
+        <v>2</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="D12" s="1">
+        <v>4</v>
+      </c>
+      <c r="E12" s="1">
+        <v>0.5</v>
+      </c>
+      <c r="F12" s="1">
+        <v>5</v>
+      </c>
+      <c r="G12" s="1">
+        <v>64</v>
+      </c>
+      <c r="H12" s="1">
+        <v>2</v>
+      </c>
+      <c r="I12" s="1">
+        <v>0.2</v>
+      </c>
+      <c r="J12" s="1">
+        <v>0.01</v>
+      </c>
+      <c r="K12" s="1">
+        <v>0.99</v>
+      </c>
+      <c r="L12" s="1">
+        <v>0.95</v>
+      </c>
+      <c r="M12" s="1">
+        <v>4000</v>
+      </c>
+      <c r="N12" s="1">
+        <v>200</v>
+      </c>
+      <c r="O12" s="1">
+        <v>2</v>
+      </c>
+      <c r="P12" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="Q12" s="1" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="13" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A13" s="1">
+        <v>10</v>
+      </c>
+      <c r="B13" s="1">
+        <v>2</v>
+      </c>
+      <c r="C13" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="D13" s="1">
+        <v>4</v>
+      </c>
+      <c r="E13" s="1">
+        <v>0.5</v>
+      </c>
+      <c r="F13" s="1">
+        <v>5</v>
+      </c>
+      <c r="G13" s="1">
+        <v>64</v>
+      </c>
+      <c r="H13" s="1">
+        <v>2</v>
+      </c>
+      <c r="I13" s="1">
+        <v>0.2</v>
+      </c>
+      <c r="J13" s="1">
+        <v>0.01</v>
+      </c>
+      <c r="K13" s="1">
+        <v>0.99</v>
+      </c>
+      <c r="L13" s="1">
+        <v>0.95</v>
+      </c>
+      <c r="M13" s="1">
+        <v>4000</v>
+      </c>
+      <c r="N13" s="1">
+        <v>200</v>
+      </c>
+      <c r="O13" s="1">
+        <v>2</v>
+      </c>
+      <c r="P13" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="Q13" s="1" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="14" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A14" s="1">
+        <v>10</v>
+      </c>
+      <c r="B14" s="1">
+        <v>2</v>
+      </c>
+      <c r="C14" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="D14" s="1">
+        <v>4</v>
+      </c>
+      <c r="E14" s="1">
+        <v>0.5</v>
+      </c>
+      <c r="F14" s="1">
+        <v>5</v>
+      </c>
+      <c r="G14" s="1">
+        <v>64</v>
+      </c>
+      <c r="H14" s="1">
+        <v>2</v>
+      </c>
+      <c r="I14" s="1">
+        <v>0.2</v>
+      </c>
+      <c r="J14" s="1">
+        <v>0.01</v>
+      </c>
+      <c r="K14" s="1">
+        <v>0.99</v>
+      </c>
+      <c r="L14" s="1">
+        <v>0.95</v>
+      </c>
+      <c r="M14" s="1">
+        <v>4000</v>
+      </c>
+      <c r="N14" s="1">
+        <v>200</v>
+      </c>
+      <c r="O14" s="1">
+        <v>2</v>
+      </c>
+      <c r="P14" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="Q14" s="1" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="15" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A15" s="1">
+        <v>11</v>
+      </c>
+      <c r="B15" s="1">
+        <v>2</v>
+      </c>
+      <c r="C15" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="D15" s="1">
+        <v>4</v>
+      </c>
+      <c r="E15" s="1">
+        <v>0.5</v>
+      </c>
+      <c r="F15" s="1">
+        <v>5</v>
+      </c>
+      <c r="G15" s="1">
+        <v>64</v>
+      </c>
+      <c r="H15" s="1">
+        <v>2</v>
+      </c>
+      <c r="I15" s="1">
+        <v>0.2</v>
+      </c>
+      <c r="J15" s="1">
+        <v>0.01</v>
+      </c>
+      <c r="K15" s="1">
+        <v>0.99</v>
+      </c>
+      <c r="L15" s="1">
+        <v>0.95</v>
+      </c>
+      <c r="M15" s="1">
+        <v>4000</v>
+      </c>
+      <c r="N15" s="1">
+        <v>200</v>
+      </c>
+      <c r="O15" s="1">
+        <v>3</v>
+      </c>
+      <c r="P15" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="Q15" s="1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="16" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A16" s="1">
+        <v>12</v>
+      </c>
+      <c r="B16" s="1">
+        <v>2</v>
+      </c>
+      <c r="C16" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="D16" s="1">
+        <v>4</v>
+      </c>
+      <c r="E16" s="1">
+        <v>0.5</v>
+      </c>
+      <c r="F16" s="1">
+        <v>5</v>
+      </c>
+      <c r="G16" s="1">
+        <v>64</v>
+      </c>
+      <c r="H16" s="1">
+        <v>2</v>
+      </c>
+      <c r="I16" s="1">
+        <v>0.2</v>
+      </c>
+      <c r="J16" s="1">
+        <v>0.01</v>
+      </c>
+      <c r="K16" s="1">
+        <v>0.99</v>
+      </c>
+      <c r="L16" s="1">
+        <v>0.95</v>
+      </c>
+      <c r="M16" s="1">
+        <v>4000</v>
+      </c>
+      <c r="N16" s="1">
+        <v>200</v>
+      </c>
+      <c r="O16" s="1">
+        <v>4</v>
+      </c>
+      <c r="P16" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="Q16" s="1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="17" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A17" s="1">
+        <v>13</v>
+      </c>
+      <c r="B17" s="1">
+        <v>2</v>
+      </c>
+      <c r="C17" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="D17" s="1">
+        <v>4</v>
+      </c>
+      <c r="E17" s="1">
+        <v>0.5</v>
+      </c>
+      <c r="F17" s="1">
+        <v>5</v>
+      </c>
+      <c r="G17" s="1">
+        <v>128</v>
+      </c>
+      <c r="H17" s="1">
+        <v>2</v>
+      </c>
+      <c r="I17" s="1">
+        <v>0.2</v>
+      </c>
+      <c r="J17" s="1">
+        <v>0.01</v>
+      </c>
+      <c r="K17" s="1">
+        <v>0.99</v>
+      </c>
+      <c r="L17" s="1">
+        <v>0.95</v>
+      </c>
+      <c r="M17" s="1">
+        <v>4000</v>
+      </c>
+      <c r="N17" s="1">
+        <v>200</v>
+      </c>
+      <c r="O17" s="1">
+        <v>2</v>
+      </c>
+      <c r="P17" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="Q17" s="1" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="18" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A18" s="1">
+        <v>14</v>
+      </c>
+      <c r="B18" s="1">
+        <v>2</v>
+      </c>
+      <c r="C18" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="D18" s="1">
+        <v>4</v>
+      </c>
+      <c r="E18" s="1">
+        <v>0.5</v>
+      </c>
+      <c r="F18" s="1">
+        <v>5</v>
+      </c>
+      <c r="G18" s="1">
+        <v>128</v>
+      </c>
+      <c r="H18" s="1">
+        <v>2</v>
+      </c>
+      <c r="I18" s="1">
+        <v>0.1</v>
+      </c>
+      <c r="J18" s="1">
+        <v>0.01</v>
+      </c>
+      <c r="K18" s="1">
+        <v>0.99</v>
+      </c>
+      <c r="L18" s="1">
+        <v>0.95</v>
+      </c>
+      <c r="M18" s="1">
+        <v>4000</v>
+      </c>
+      <c r="N18" s="1">
+        <v>200</v>
+      </c>
+      <c r="O18" s="1">
+        <v>2</v>
+      </c>
+      <c r="P18" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="Q18" s="1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="19" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A19" s="1">
+        <v>15</v>
+      </c>
+      <c r="B19" s="1">
+        <v>2</v>
+      </c>
+      <c r="C19" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="D19" s="1">
+        <v>4</v>
+      </c>
+      <c r="E19" s="1">
+        <v>0.5</v>
+      </c>
+      <c r="F19" s="1">
+        <v>5</v>
+      </c>
+      <c r="G19" s="1">
+        <v>128</v>
+      </c>
+      <c r="H19" s="1">
+        <v>2</v>
+      </c>
+      <c r="I19" s="1">
+        <v>0.1</v>
+      </c>
+      <c r="J19" s="1">
+        <v>1.4999999999999999E-2</v>
+      </c>
+      <c r="K19" s="1">
+        <v>0.99</v>
+      </c>
+      <c r="L19" s="1">
+        <v>0.95</v>
+      </c>
+      <c r="M19" s="1">
+        <v>4000</v>
+      </c>
+      <c r="N19" s="1">
+        <v>200</v>
+      </c>
+      <c r="O19" s="1">
+        <v>2</v>
+      </c>
+      <c r="P19" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="Q19" s="1" t="s">
+        <v>18</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updates to Trial 15 and 16
</commit_message>
<xml_diff>
--- a/documentation/trials.xlsx
+++ b/documentation/trials.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ocean\Documents\GitHub\CPTS-437-DDPG-RSSI-Car\documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{34E2F94F-A29A-45A2-8211-0B8EE7D3A184}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2DD2B046-DF8B-47D5-9D1E-A268F87CA0D8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{496E26A4-E262-4A0D-A9DD-90AD4307AC27}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="31">
   <si>
     <t>memory_size</t>
   </si>
@@ -123,6 +123,12 @@
   </si>
   <si>
     <t>target_kl</t>
+  </si>
+  <si>
+    <t>vf_lr</t>
+  </si>
+  <si>
+    <t>Bad at 200 and 1000</t>
   </si>
 </sst>
 </file>
@@ -158,9 +164,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -497,10 +506,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DD51C088-492E-456A-BAA7-804EE5452A68}">
-  <dimension ref="A1:Q19"/>
+  <dimension ref="A1:R21"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="Q20" sqref="Q20"/>
+    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
+      <selection activeCell="S13" sqref="S13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -511,15 +520,15 @@
     <col min="4" max="5" width="25.88671875" style="1" bestFit="1" customWidth="1"/>
     <col min="6" max="7" width="13.88671875" style="1" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="14.6640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="9" max="10" width="14.6640625" style="1" customWidth="1"/>
-    <col min="11" max="11" width="14.6640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="12" max="15" width="14.5546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="9.77734375" style="1" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="15.88671875" style="1" bestFit="1" customWidth="1"/>
-    <col min="18" max="16384" width="8.88671875" style="1"/>
+    <col min="9" max="11" width="14.6640625" style="1" customWidth="1"/>
+    <col min="12" max="12" width="14.6640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="13" max="16" width="14.5546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="9.77734375" style="1" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="17.21875" style="1" bestFit="1" customWidth="1"/>
+    <col min="19" max="16384" width="8.88671875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>6</v>
       </c>
@@ -548,31 +557,34 @@
         <v>27</v>
       </c>
       <c r="J1" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="K1" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="L1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="L1" s="1" t="s">
+      <c r="M1" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="M1" s="1" t="s">
-        <v>4</v>
-      </c>
       <c r="N1" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="O1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="P1" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="P1" s="1" t="s">
+      <c r="Q1" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="Q1" s="1" t="s">
+      <c r="R1" s="1" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="2" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A2" s="1">
         <v>1</v>
       </c>
@@ -600,32 +612,35 @@
       <c r="I2" s="1">
         <v>0.2</v>
       </c>
-      <c r="J2" s="1">
+      <c r="J2" s="2">
+        <v>1E-3</v>
+      </c>
+      <c r="K2" s="1">
         <v>0.01</v>
       </c>
-      <c r="K2" s="1">
+      <c r="L2" s="1">
         <v>0.99</v>
       </c>
-      <c r="L2" s="1">
-        <v>0.95</v>
-      </c>
       <c r="M2" s="1">
-        <v>4000</v>
+        <v>0.95</v>
       </c>
       <c r="N2" s="1">
+        <v>4000</v>
+      </c>
+      <c r="O2" s="1">
         <v>1000</v>
       </c>
-      <c r="O2" s="1">
+      <c r="P2" s="1">
         <v>1</v>
       </c>
-      <c r="P2" s="1" t="s">
-        <v>9</v>
-      </c>
       <c r="Q2" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="R2" s="1" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="3" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A3" s="1">
         <v>2</v>
       </c>
@@ -653,32 +668,35 @@
       <c r="I3" s="1">
         <v>0.2</v>
       </c>
-      <c r="J3" s="1">
+      <c r="J3" s="2">
+        <v>1E-3</v>
+      </c>
+      <c r="K3" s="1">
         <v>0.01</v>
       </c>
-      <c r="K3" s="1">
+      <c r="L3" s="1">
         <v>0.99</v>
       </c>
-      <c r="L3" s="1">
-        <v>0.95</v>
-      </c>
       <c r="M3" s="1">
-        <v>4000</v>
+        <v>0.95</v>
       </c>
       <c r="N3" s="1">
+        <v>4000</v>
+      </c>
+      <c r="O3" s="1">
         <v>1000</v>
       </c>
-      <c r="O3" s="1">
+      <c r="P3" s="1">
         <v>1</v>
       </c>
-      <c r="P3" s="1" t="s">
-        <v>9</v>
-      </c>
       <c r="Q3" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="R3" s="1" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="4" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A4" s="1">
         <v>3</v>
       </c>
@@ -706,29 +724,32 @@
       <c r="I4" s="1">
         <v>0.2</v>
       </c>
-      <c r="J4" s="1">
+      <c r="J4" s="2">
+        <v>1E-3</v>
+      </c>
+      <c r="K4" s="1">
         <v>0.01</v>
       </c>
-      <c r="K4" s="1">
+      <c r="L4" s="1">
         <v>0.99</v>
       </c>
-      <c r="L4" s="1">
-        <v>0.95</v>
-      </c>
       <c r="M4" s="1">
-        <v>4000</v>
+        <v>0.95</v>
       </c>
       <c r="N4" s="1">
+        <v>4000</v>
+      </c>
+      <c r="O4" s="1">
         <v>1000</v>
       </c>
-      <c r="O4" s="1">
+      <c r="P4" s="1">
         <v>1</v>
       </c>
-      <c r="P4" s="1" t="s">
+      <c r="Q4" s="1" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="5" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A5" s="1">
         <v>4</v>
       </c>
@@ -756,32 +777,35 @@
       <c r="I5" s="1">
         <v>0.2</v>
       </c>
-      <c r="J5" s="1">
+      <c r="J5" s="2">
+        <v>1E-3</v>
+      </c>
+      <c r="K5" s="1">
         <v>0.01</v>
       </c>
-      <c r="K5" s="1">
+      <c r="L5" s="1">
         <v>0.99</v>
       </c>
-      <c r="L5" s="1">
-        <v>0.95</v>
-      </c>
       <c r="M5" s="1">
-        <v>4000</v>
+        <v>0.95</v>
       </c>
       <c r="N5" s="1">
+        <v>4000</v>
+      </c>
+      <c r="O5" s="1">
         <v>1000</v>
       </c>
-      <c r="O5" s="1">
+      <c r="P5" s="1">
         <v>1</v>
       </c>
-      <c r="P5" s="1" t="s">
-        <v>10</v>
-      </c>
       <c r="Q5" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="R5" s="1" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="6" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A6" s="1">
         <v>5</v>
       </c>
@@ -809,32 +833,35 @@
       <c r="I6" s="1">
         <v>0.2</v>
       </c>
-      <c r="J6" s="1">
+      <c r="J6" s="2">
+        <v>1E-3</v>
+      </c>
+      <c r="K6" s="1">
         <v>0.01</v>
       </c>
-      <c r="K6" s="1">
+      <c r="L6" s="1">
         <v>0.99</v>
       </c>
-      <c r="L6" s="1">
-        <v>0.95</v>
-      </c>
       <c r="M6" s="1">
-        <v>4000</v>
+        <v>0.95</v>
       </c>
       <c r="N6" s="1">
+        <v>4000</v>
+      </c>
+      <c r="O6" s="1">
         <v>1000</v>
       </c>
-      <c r="O6" s="1">
+      <c r="P6" s="1">
         <v>1</v>
       </c>
-      <c r="P6" s="1" t="s">
-        <v>9</v>
-      </c>
       <c r="Q6" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="R6" s="1" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="7" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A7" s="1">
         <v>6</v>
       </c>
@@ -862,32 +889,35 @@
       <c r="I7" s="1">
         <v>0.2</v>
       </c>
-      <c r="J7" s="1">
+      <c r="J7" s="2">
+        <v>1E-3</v>
+      </c>
+      <c r="K7" s="1">
         <v>0.01</v>
       </c>
-      <c r="K7" s="1">
-        <v>0.95</v>
-      </c>
       <c r="L7" s="1">
         <v>0.95</v>
       </c>
       <c r="M7" s="1">
-        <v>4000</v>
+        <v>0.95</v>
       </c>
       <c r="N7" s="1">
+        <v>4000</v>
+      </c>
+      <c r="O7" s="1">
         <v>1000</v>
       </c>
-      <c r="O7" s="1">
+      <c r="P7" s="1">
         <v>1</v>
       </c>
-      <c r="P7" s="1" t="s">
-        <v>10</v>
-      </c>
       <c r="Q7" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="R7" s="1" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="8" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A8" s="1">
         <v>7</v>
       </c>
@@ -915,32 +945,35 @@
       <c r="I8" s="1">
         <v>0.2</v>
       </c>
-      <c r="J8" s="1">
+      <c r="J8" s="2">
+        <v>1E-3</v>
+      </c>
+      <c r="K8" s="1">
         <v>0.01</v>
       </c>
-      <c r="K8" s="1">
+      <c r="L8" s="1">
         <v>0.9</v>
       </c>
-      <c r="L8" s="1">
-        <v>0.95</v>
-      </c>
       <c r="M8" s="1">
-        <v>4000</v>
+        <v>0.95</v>
       </c>
       <c r="N8" s="1">
+        <v>4000</v>
+      </c>
+      <c r="O8" s="1">
         <v>1000</v>
       </c>
-      <c r="O8" s="1">
+      <c r="P8" s="1">
         <v>1</v>
       </c>
-      <c r="P8" s="1" t="s">
-        <v>10</v>
-      </c>
       <c r="Q8" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="R8" s="1" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="9" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A9" s="1">
         <v>8</v>
       </c>
@@ -968,32 +1001,35 @@
       <c r="I9" s="1">
         <v>0.2</v>
       </c>
-      <c r="J9" s="1">
+      <c r="J9" s="2">
+        <v>1E-3</v>
+      </c>
+      <c r="K9" s="1">
         <v>0.01</v>
       </c>
-      <c r="K9" s="1">
+      <c r="L9" s="1">
         <v>0.99</v>
       </c>
-      <c r="L9" s="1">
-        <v>0.95</v>
-      </c>
       <c r="M9" s="1">
-        <v>4000</v>
+        <v>0.95</v>
       </c>
       <c r="N9" s="1">
+        <v>4000</v>
+      </c>
+      <c r="O9" s="1">
         <v>200</v>
       </c>
-      <c r="O9" s="1">
-        <v>2</v>
-      </c>
-      <c r="P9" s="1" t="s">
-        <v>9</v>
+      <c r="P9" s="1">
+        <v>2</v>
       </c>
       <c r="Q9" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="R9" s="1" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="10" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A10" s="1">
         <v>8</v>
       </c>
@@ -1021,32 +1057,35 @@
       <c r="I10" s="1">
         <v>0.2</v>
       </c>
-      <c r="J10" s="1">
+      <c r="J10" s="2">
+        <v>1E-3</v>
+      </c>
+      <c r="K10" s="1">
         <v>0.01</v>
       </c>
-      <c r="K10" s="1">
+      <c r="L10" s="1">
         <v>0.99</v>
       </c>
-      <c r="L10" s="1">
-        <v>0.95</v>
-      </c>
       <c r="M10" s="1">
-        <v>4000</v>
+        <v>0.95</v>
       </c>
       <c r="N10" s="1">
+        <v>4000</v>
+      </c>
+      <c r="O10" s="1">
         <v>200</v>
       </c>
-      <c r="O10" s="1">
-        <v>2</v>
-      </c>
-      <c r="P10" s="1" t="s">
-        <v>9</v>
+      <c r="P10" s="1">
+        <v>2</v>
       </c>
       <c r="Q10" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="R10" s="1" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="11" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A11" s="1">
         <v>9</v>
       </c>
@@ -1074,32 +1113,35 @@
       <c r="I11" s="1">
         <v>0.2</v>
       </c>
-      <c r="J11" s="1">
+      <c r="J11" s="2">
+        <v>1E-3</v>
+      </c>
+      <c r="K11" s="1">
         <v>0.01</v>
       </c>
-      <c r="K11" s="1">
+      <c r="L11" s="1">
         <v>0.99</v>
       </c>
-      <c r="L11" s="1">
-        <v>0.95</v>
-      </c>
       <c r="M11" s="1">
-        <v>4000</v>
+        <v>0.95</v>
       </c>
       <c r="N11" s="1">
+        <v>4000</v>
+      </c>
+      <c r="O11" s="1">
         <v>200</v>
       </c>
-      <c r="O11" s="1">
-        <v>2</v>
-      </c>
-      <c r="P11" s="1" t="s">
-        <v>9</v>
+      <c r="P11" s="1">
+        <v>2</v>
       </c>
       <c r="Q11" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="R11" s="1" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="12" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A12" s="1">
         <v>10</v>
       </c>
@@ -1127,32 +1169,35 @@
       <c r="I12" s="1">
         <v>0.2</v>
       </c>
-      <c r="J12" s="1">
+      <c r="J12" s="2">
+        <v>1E-3</v>
+      </c>
+      <c r="K12" s="1">
         <v>0.01</v>
       </c>
-      <c r="K12" s="1">
+      <c r="L12" s="1">
         <v>0.99</v>
       </c>
-      <c r="L12" s="1">
-        <v>0.95</v>
-      </c>
       <c r="M12" s="1">
-        <v>4000</v>
+        <v>0.95</v>
       </c>
       <c r="N12" s="1">
+        <v>4000</v>
+      </c>
+      <c r="O12" s="1">
         <v>200</v>
       </c>
-      <c r="O12" s="1">
-        <v>2</v>
-      </c>
-      <c r="P12" s="1" t="s">
-        <v>9</v>
+      <c r="P12" s="1">
+        <v>2</v>
       </c>
       <c r="Q12" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="R12" s="1" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="13" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A13" s="1">
         <v>10</v>
       </c>
@@ -1180,32 +1225,35 @@
       <c r="I13" s="1">
         <v>0.2</v>
       </c>
-      <c r="J13" s="1">
+      <c r="J13" s="2">
+        <v>1E-3</v>
+      </c>
+      <c r="K13" s="1">
         <v>0.01</v>
       </c>
-      <c r="K13" s="1">
+      <c r="L13" s="1">
         <v>0.99</v>
       </c>
-      <c r="L13" s="1">
-        <v>0.95</v>
-      </c>
       <c r="M13" s="1">
-        <v>4000</v>
+        <v>0.95</v>
       </c>
       <c r="N13" s="1">
+        <v>4000</v>
+      </c>
+      <c r="O13" s="1">
         <v>200</v>
       </c>
-      <c r="O13" s="1">
-        <v>2</v>
-      </c>
-      <c r="P13" s="1" t="s">
-        <v>9</v>
+      <c r="P13" s="1">
+        <v>2</v>
       </c>
       <c r="Q13" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="R13" s="1" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="14" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A14" s="1">
         <v>10</v>
       </c>
@@ -1233,32 +1281,35 @@
       <c r="I14" s="1">
         <v>0.2</v>
       </c>
-      <c r="J14" s="1">
+      <c r="J14" s="2">
+        <v>1E-3</v>
+      </c>
+      <c r="K14" s="1">
         <v>0.01</v>
       </c>
-      <c r="K14" s="1">
+      <c r="L14" s="1">
         <v>0.99</v>
       </c>
-      <c r="L14" s="1">
-        <v>0.95</v>
-      </c>
       <c r="M14" s="1">
-        <v>4000</v>
+        <v>0.95</v>
       </c>
       <c r="N14" s="1">
+        <v>4000</v>
+      </c>
+      <c r="O14" s="1">
         <v>200</v>
       </c>
-      <c r="O14" s="1">
-        <v>2</v>
-      </c>
-      <c r="P14" s="1" t="s">
-        <v>9</v>
+      <c r="P14" s="1">
+        <v>2</v>
       </c>
       <c r="Q14" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="R14" s="1" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="15" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A15" s="1">
         <v>11</v>
       </c>
@@ -1286,32 +1337,35 @@
       <c r="I15" s="1">
         <v>0.2</v>
       </c>
-      <c r="J15" s="1">
+      <c r="J15" s="2">
+        <v>1E-3</v>
+      </c>
+      <c r="K15" s="1">
         <v>0.01</v>
       </c>
-      <c r="K15" s="1">
+      <c r="L15" s="1">
         <v>0.99</v>
       </c>
-      <c r="L15" s="1">
-        <v>0.95</v>
-      </c>
       <c r="M15" s="1">
-        <v>4000</v>
+        <v>0.95</v>
       </c>
       <c r="N15" s="1">
+        <v>4000</v>
+      </c>
+      <c r="O15" s="1">
         <v>200</v>
       </c>
-      <c r="O15" s="1">
+      <c r="P15" s="1">
         <v>3</v>
       </c>
-      <c r="P15" s="1" t="s">
-        <v>9</v>
-      </c>
       <c r="Q15" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="R15" s="1" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="16" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A16" s="1">
         <v>12</v>
       </c>
@@ -1339,32 +1393,35 @@
       <c r="I16" s="1">
         <v>0.2</v>
       </c>
-      <c r="J16" s="1">
+      <c r="J16" s="2">
+        <v>1E-3</v>
+      </c>
+      <c r="K16" s="1">
         <v>0.01</v>
       </c>
-      <c r="K16" s="1">
+      <c r="L16" s="1">
         <v>0.99</v>
       </c>
-      <c r="L16" s="1">
-        <v>0.95</v>
-      </c>
       <c r="M16" s="1">
-        <v>4000</v>
+        <v>0.95</v>
       </c>
       <c r="N16" s="1">
+        <v>4000</v>
+      </c>
+      <c r="O16" s="1">
         <v>200</v>
       </c>
-      <c r="O16" s="1">
-        <v>4</v>
-      </c>
-      <c r="P16" s="1" t="s">
-        <v>9</v>
+      <c r="P16" s="1">
+        <v>4</v>
       </c>
       <c r="Q16" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="R16" s="1" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="17" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A17" s="1">
         <v>13</v>
       </c>
@@ -1392,32 +1449,35 @@
       <c r="I17" s="1">
         <v>0.2</v>
       </c>
-      <c r="J17" s="1">
+      <c r="J17" s="2">
+        <v>1E-3</v>
+      </c>
+      <c r="K17" s="1">
         <v>0.01</v>
       </c>
-      <c r="K17" s="1">
+      <c r="L17" s="1">
         <v>0.99</v>
       </c>
-      <c r="L17" s="1">
-        <v>0.95</v>
-      </c>
       <c r="M17" s="1">
-        <v>4000</v>
+        <v>0.95</v>
       </c>
       <c r="N17" s="1">
+        <v>4000</v>
+      </c>
+      <c r="O17" s="1">
         <v>200</v>
       </c>
-      <c r="O17" s="1">
-        <v>2</v>
-      </c>
-      <c r="P17" s="1" t="s">
-        <v>9</v>
+      <c r="P17" s="1">
+        <v>2</v>
       </c>
       <c r="Q17" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="R17" s="1" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="18" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A18" s="1">
         <v>14</v>
       </c>
@@ -1445,32 +1505,35 @@
       <c r="I18" s="1">
         <v>0.1</v>
       </c>
-      <c r="J18" s="1">
+      <c r="J18" s="2">
+        <v>1E-3</v>
+      </c>
+      <c r="K18" s="1">
         <v>0.01</v>
       </c>
-      <c r="K18" s="1">
+      <c r="L18" s="1">
         <v>0.99</v>
       </c>
-      <c r="L18" s="1">
-        <v>0.95</v>
-      </c>
       <c r="M18" s="1">
-        <v>4000</v>
+        <v>0.95</v>
       </c>
       <c r="N18" s="1">
+        <v>4000</v>
+      </c>
+      <c r="O18" s="1">
         <v>200</v>
       </c>
-      <c r="O18" s="1">
-        <v>2</v>
-      </c>
-      <c r="P18" s="1" t="s">
-        <v>9</v>
+      <c r="P18" s="1">
+        <v>2</v>
       </c>
       <c r="Q18" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="R18" s="1" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="19" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A19" s="1">
         <v>15</v>
       </c>
@@ -1498,29 +1561,144 @@
       <c r="I19" s="1">
         <v>0.1</v>
       </c>
-      <c r="J19" s="1">
+      <c r="J19" s="2">
+        <v>1E-3</v>
+      </c>
+      <c r="K19" s="1">
         <v>1.4999999999999999E-2</v>
       </c>
-      <c r="K19" s="1">
+      <c r="L19" s="1">
         <v>0.99</v>
       </c>
-      <c r="L19" s="1">
-        <v>0.95</v>
-      </c>
       <c r="M19" s="1">
-        <v>4000</v>
+        <v>0.95</v>
       </c>
       <c r="N19" s="1">
+        <v>4000</v>
+      </c>
+      <c r="O19" s="1">
         <v>200</v>
       </c>
-      <c r="O19" s="1">
-        <v>2</v>
-      </c>
-      <c r="P19" s="1" t="s">
-        <v>9</v>
+      <c r="P19" s="1">
+        <v>2</v>
       </c>
       <c r="Q19" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="R19" s="1" t="s">
         <v>18</v>
+      </c>
+    </row>
+    <row r="20" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A20" s="1">
+        <v>15</v>
+      </c>
+      <c r="B20" s="1">
+        <v>2</v>
+      </c>
+      <c r="C20" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="D20" s="1">
+        <v>4</v>
+      </c>
+      <c r="E20" s="1">
+        <v>0.5</v>
+      </c>
+      <c r="F20" s="1">
+        <v>5</v>
+      </c>
+      <c r="G20" s="1">
+        <v>128</v>
+      </c>
+      <c r="H20" s="1">
+        <v>2</v>
+      </c>
+      <c r="I20" s="1">
+        <v>0.1</v>
+      </c>
+      <c r="J20" s="2">
+        <v>1E-3</v>
+      </c>
+      <c r="K20" s="1">
+        <v>1.4999999999999999E-2</v>
+      </c>
+      <c r="L20" s="1">
+        <v>0.99</v>
+      </c>
+      <c r="M20" s="1">
+        <v>0.95</v>
+      </c>
+      <c r="N20" s="1">
+        <v>4000</v>
+      </c>
+      <c r="O20" s="1">
+        <v>800</v>
+      </c>
+      <c r="P20" s="1">
+        <v>2</v>
+      </c>
+      <c r="Q20" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="R20" s="1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="21" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A21" s="1">
+        <v>16</v>
+      </c>
+      <c r="B21" s="1">
+        <v>2</v>
+      </c>
+      <c r="C21" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="D21" s="1">
+        <v>4</v>
+      </c>
+      <c r="E21" s="1">
+        <v>0.5</v>
+      </c>
+      <c r="F21" s="1">
+        <v>5</v>
+      </c>
+      <c r="G21" s="1">
+        <v>128</v>
+      </c>
+      <c r="H21" s="1">
+        <v>2</v>
+      </c>
+      <c r="I21" s="1">
+        <v>0.1</v>
+      </c>
+      <c r="J21" s="2">
+        <v>5.0000000000000001E-4</v>
+      </c>
+      <c r="K21" s="1">
+        <v>1.4999999999999999E-2</v>
+      </c>
+      <c r="L21" s="1">
+        <v>0.99</v>
+      </c>
+      <c r="M21" s="1">
+        <v>0.95</v>
+      </c>
+      <c r="N21" s="1">
+        <v>4000</v>
+      </c>
+      <c r="O21" s="1">
+        <v>1000</v>
+      </c>
+      <c r="P21" s="1">
+        <v>2</v>
+      </c>
+      <c r="Q21" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="R21" s="1" t="s">
+        <v>30</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added trial 17 (great results)
</commit_message>
<xml_diff>
--- a/documentation/trials.xlsx
+++ b/documentation/trials.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ocean\Documents\GitHub\CPTS-437-DDPG-RSSI-Car\documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2DD2B046-DF8B-47D5-9D1E-A268F87CA0D8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BA3D0B27-FDF7-407E-BFAE-6A6DD6E9B94B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{496E26A4-E262-4A0D-A9DD-90AD4307AC27}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="35">
   <si>
     <t>memory_size</t>
   </si>
@@ -129,12 +129,27 @@
   </si>
   <si>
     <t>Bad at 200 and 1000</t>
+  </si>
+  <si>
+    <t>pi_lr</t>
+  </si>
+  <si>
+    <t>max_ep_len</t>
+  </si>
+  <si>
+    <t>Good results. Still crashes a lot. Might want to try increasing crash penalty afterwards. I think I should keep on training this model.</t>
+  </si>
+  <si>
+    <t>Not so good. It got maybe slightly better but the training is so unstable that I should stop.</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="0E+00"/>
+  </numFmts>
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -164,13 +179,16 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -506,10 +524,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DD51C088-492E-456A-BAA7-804EE5452A68}">
-  <dimension ref="A1:R21"/>
+  <dimension ref="A1:T24"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
-      <selection activeCell="S13" sqref="S13"/>
+    <sheetView tabSelected="1" topLeftCell="A11" workbookViewId="0">
+      <selection activeCell="E24" sqref="E24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -518,17 +536,18 @@
     <col min="2" max="2" width="14.6640625" style="1" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="15.109375" style="1" bestFit="1" customWidth="1"/>
     <col min="4" max="5" width="25.88671875" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="7" width="13.88671875" style="1" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="14.6640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="9" max="11" width="14.6640625" style="1" customWidth="1"/>
-    <col min="12" max="12" width="14.6640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="13" max="16" width="14.5546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="9.77734375" style="1" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="17.21875" style="1" bestFit="1" customWidth="1"/>
-    <col min="19" max="16384" width="8.88671875" style="1"/>
+    <col min="6" max="6" width="25.88671875" style="1" customWidth="1"/>
+    <col min="7" max="8" width="13.88671875" style="1" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="14.6640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="10" max="13" width="14.6640625" style="1" customWidth="1"/>
+    <col min="14" max="14" width="14.6640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="15" max="18" width="14.5546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="9.77734375" style="1" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="34.109375" style="3" customWidth="1"/>
+    <col min="21" max="16384" width="8.88671875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>6</v>
       </c>
@@ -545,46 +564,52 @@
         <v>14</v>
       </c>
       <c r="F1" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="G1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="H1" s="1" t="s">
-        <v>2</v>
-      </c>
       <c r="I1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="J1" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="K1" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="L1" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="M1" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="L1" s="1" t="s">
+      <c r="N1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="M1" s="1" t="s">
+      <c r="O1" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="N1" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="O1" s="1" t="s">
-        <v>5</v>
-      </c>
       <c r="P1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="Q1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="R1" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="Q1" s="1" t="s">
+      <c r="S1" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="R1" s="1" t="s">
+      <c r="T1" s="3" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="2" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A2" s="1">
         <v>1</v>
       </c>
@@ -601,46 +626,52 @@
         <v>0.5</v>
       </c>
       <c r="F2" s="1">
+        <v>1000</v>
+      </c>
+      <c r="G2" s="1">
         <v>10</v>
       </c>
-      <c r="G2" s="1">
+      <c r="H2" s="1">
         <v>128</v>
       </c>
-      <c r="H2" s="1">
+      <c r="I2" s="1">
         <v>3</v>
       </c>
-      <c r="I2" s="1">
+      <c r="J2" s="1">
         <v>0.2</v>
       </c>
-      <c r="J2" s="2">
-        <v>1E-3</v>
-      </c>
-      <c r="K2" s="1">
+      <c r="K2" s="2">
+        <v>2.9999999999999997E-4</v>
+      </c>
+      <c r="L2" s="2">
+        <v>1E-3</v>
+      </c>
+      <c r="M2" s="1">
         <v>0.01</v>
       </c>
-      <c r="L2" s="1">
+      <c r="N2" s="1">
         <v>0.99</v>
       </c>
-      <c r="M2" s="1">
-        <v>0.95</v>
-      </c>
-      <c r="N2" s="1">
-        <v>4000</v>
-      </c>
       <c r="O2" s="1">
-        <v>1000</v>
+        <v>0.95</v>
       </c>
       <c r="P2" s="1">
+        <v>4000</v>
+      </c>
+      <c r="Q2" s="1">
+        <v>1000</v>
+      </c>
+      <c r="R2" s="1">
         <v>1</v>
       </c>
-      <c r="Q2" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="R2" s="1" t="s">
+      <c r="S2" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="T2" s="3" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="3" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A3" s="1">
         <v>2</v>
       </c>
@@ -657,46 +688,52 @@
         <v>0.5</v>
       </c>
       <c r="F3" s="1">
+        <v>1000</v>
+      </c>
+      <c r="G3" s="1">
         <v>10</v>
       </c>
-      <c r="G3" s="1">
+      <c r="H3" s="1">
         <v>128</v>
       </c>
-      <c r="H3" s="1">
+      <c r="I3" s="1">
         <v>3</v>
       </c>
-      <c r="I3" s="1">
+      <c r="J3" s="1">
         <v>0.2</v>
       </c>
-      <c r="J3" s="2">
-        <v>1E-3</v>
-      </c>
-      <c r="K3" s="1">
+      <c r="K3" s="2">
+        <v>2.9999999999999997E-4</v>
+      </c>
+      <c r="L3" s="2">
+        <v>1E-3</v>
+      </c>
+      <c r="M3" s="1">
         <v>0.01</v>
       </c>
-      <c r="L3" s="1">
+      <c r="N3" s="1">
         <v>0.99</v>
       </c>
-      <c r="M3" s="1">
-        <v>0.95</v>
-      </c>
-      <c r="N3" s="1">
-        <v>4000</v>
-      </c>
       <c r="O3" s="1">
-        <v>1000</v>
+        <v>0.95</v>
       </c>
       <c r="P3" s="1">
+        <v>4000</v>
+      </c>
+      <c r="Q3" s="1">
+        <v>1000</v>
+      </c>
+      <c r="R3" s="1">
         <v>1</v>
       </c>
-      <c r="Q3" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="R3" s="1" t="s">
+      <c r="S3" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="T3" s="3" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="4" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A4" s="1">
         <v>3</v>
       </c>
@@ -713,43 +750,49 @@
         <v>0.5</v>
       </c>
       <c r="F4" s="1">
-        <v>5</v>
+        <v>1000</v>
       </c>
       <c r="G4" s="1">
+        <v>5</v>
+      </c>
+      <c r="H4" s="1">
         <v>128</v>
       </c>
-      <c r="H4" s="1">
+      <c r="I4" s="1">
         <v>3</v>
       </c>
-      <c r="I4" s="1">
+      <c r="J4" s="1">
         <v>0.2</v>
       </c>
-      <c r="J4" s="2">
-        <v>1E-3</v>
-      </c>
-      <c r="K4" s="1">
+      <c r="K4" s="2">
+        <v>2.9999999999999997E-4</v>
+      </c>
+      <c r="L4" s="2">
+        <v>1E-3</v>
+      </c>
+      <c r="M4" s="1">
         <v>0.01</v>
       </c>
-      <c r="L4" s="1">
+      <c r="N4" s="1">
         <v>0.99</v>
       </c>
-      <c r="M4" s="1">
-        <v>0.95</v>
-      </c>
-      <c r="N4" s="1">
-        <v>4000</v>
-      </c>
       <c r="O4" s="1">
-        <v>1000</v>
+        <v>0.95</v>
       </c>
       <c r="P4" s="1">
+        <v>4000</v>
+      </c>
+      <c r="Q4" s="1">
+        <v>1000</v>
+      </c>
+      <c r="R4" s="1">
         <v>1</v>
       </c>
-      <c r="Q4" s="1" t="s">
+      <c r="S4" s="1" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="5" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A5" s="1">
         <v>4</v>
       </c>
@@ -766,46 +809,52 @@
         <v>0.5</v>
       </c>
       <c r="F5" s="1">
+        <v>1000</v>
+      </c>
+      <c r="G5" s="1">
         <v>1</v>
       </c>
-      <c r="G5" s="1">
+      <c r="H5" s="1">
         <v>128</v>
       </c>
-      <c r="H5" s="1">
+      <c r="I5" s="1">
         <v>3</v>
       </c>
-      <c r="I5" s="1">
+      <c r="J5" s="1">
         <v>0.2</v>
       </c>
-      <c r="J5" s="2">
-        <v>1E-3</v>
-      </c>
-      <c r="K5" s="1">
+      <c r="K5" s="2">
+        <v>2.9999999999999997E-4</v>
+      </c>
+      <c r="L5" s="2">
+        <v>1E-3</v>
+      </c>
+      <c r="M5" s="1">
         <v>0.01</v>
       </c>
-      <c r="L5" s="1">
+      <c r="N5" s="1">
         <v>0.99</v>
       </c>
-      <c r="M5" s="1">
-        <v>0.95</v>
-      </c>
-      <c r="N5" s="1">
-        <v>4000</v>
-      </c>
       <c r="O5" s="1">
-        <v>1000</v>
+        <v>0.95</v>
       </c>
       <c r="P5" s="1">
+        <v>4000</v>
+      </c>
+      <c r="Q5" s="1">
+        <v>1000</v>
+      </c>
+      <c r="R5" s="1">
         <v>1</v>
       </c>
-      <c r="Q5" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="R5" s="1" t="s">
+      <c r="S5" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="T5" s="3" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="6" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A6" s="1">
         <v>5</v>
       </c>
@@ -822,46 +871,52 @@
         <v>0.5</v>
       </c>
       <c r="F6" s="1">
-        <v>5</v>
+        <v>1000</v>
       </c>
       <c r="G6" s="1">
+        <v>5</v>
+      </c>
+      <c r="H6" s="1">
         <v>64</v>
       </c>
-      <c r="H6" s="1">
-        <v>2</v>
-      </c>
       <c r="I6" s="1">
+        <v>2</v>
+      </c>
+      <c r="J6" s="1">
         <v>0.2</v>
       </c>
-      <c r="J6" s="2">
-        <v>1E-3</v>
-      </c>
-      <c r="K6" s="1">
+      <c r="K6" s="2">
+        <v>2.9999999999999997E-4</v>
+      </c>
+      <c r="L6" s="2">
+        <v>1E-3</v>
+      </c>
+      <c r="M6" s="1">
         <v>0.01</v>
       </c>
-      <c r="L6" s="1">
+      <c r="N6" s="1">
         <v>0.99</v>
       </c>
-      <c r="M6" s="1">
-        <v>0.95</v>
-      </c>
-      <c r="N6" s="1">
-        <v>4000</v>
-      </c>
       <c r="O6" s="1">
-        <v>1000</v>
+        <v>0.95</v>
       </c>
       <c r="P6" s="1">
+        <v>4000</v>
+      </c>
+      <c r="Q6" s="1">
+        <v>1000</v>
+      </c>
+      <c r="R6" s="1">
         <v>1</v>
       </c>
-      <c r="Q6" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="R6" s="1" t="s">
+      <c r="S6" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="T6" s="3" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="7" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A7" s="1">
         <v>6</v>
       </c>
@@ -878,46 +933,52 @@
         <v>0.5</v>
       </c>
       <c r="F7" s="1">
-        <v>5</v>
+        <v>1000</v>
       </c>
       <c r="G7" s="1">
+        <v>5</v>
+      </c>
+      <c r="H7" s="1">
         <v>64</v>
       </c>
-      <c r="H7" s="1">
-        <v>2</v>
-      </c>
       <c r="I7" s="1">
+        <v>2</v>
+      </c>
+      <c r="J7" s="1">
         <v>0.2</v>
       </c>
-      <c r="J7" s="2">
-        <v>1E-3</v>
-      </c>
-      <c r="K7" s="1">
+      <c r="K7" s="2">
+        <v>2.9999999999999997E-4</v>
+      </c>
+      <c r="L7" s="2">
+        <v>1E-3</v>
+      </c>
+      <c r="M7" s="1">
         <v>0.01</v>
       </c>
-      <c r="L7" s="1">
-        <v>0.95</v>
-      </c>
-      <c r="M7" s="1">
-        <v>0.95</v>
-      </c>
       <c r="N7" s="1">
-        <v>4000</v>
+        <v>0.95</v>
       </c>
       <c r="O7" s="1">
-        <v>1000</v>
+        <v>0.95</v>
       </c>
       <c r="P7" s="1">
+        <v>4000</v>
+      </c>
+      <c r="Q7" s="1">
+        <v>1000</v>
+      </c>
+      <c r="R7" s="1">
         <v>1</v>
       </c>
-      <c r="Q7" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="R7" s="1" t="s">
+      <c r="S7" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="T7" s="3" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="8" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A8" s="1">
         <v>7</v>
       </c>
@@ -934,46 +995,52 @@
         <v>0.5</v>
       </c>
       <c r="F8" s="1">
-        <v>5</v>
+        <v>1000</v>
       </c>
       <c r="G8" s="1">
+        <v>5</v>
+      </c>
+      <c r="H8" s="1">
         <v>64</v>
       </c>
-      <c r="H8" s="1">
-        <v>2</v>
-      </c>
       <c r="I8" s="1">
+        <v>2</v>
+      </c>
+      <c r="J8" s="1">
         <v>0.2</v>
       </c>
-      <c r="J8" s="2">
-        <v>1E-3</v>
-      </c>
-      <c r="K8" s="1">
+      <c r="K8" s="2">
+        <v>2.9999999999999997E-4</v>
+      </c>
+      <c r="L8" s="2">
+        <v>1E-3</v>
+      </c>
+      <c r="M8" s="1">
         <v>0.01</v>
       </c>
-      <c r="L8" s="1">
+      <c r="N8" s="1">
         <v>0.9</v>
       </c>
-      <c r="M8" s="1">
-        <v>0.95</v>
-      </c>
-      <c r="N8" s="1">
-        <v>4000</v>
-      </c>
       <c r="O8" s="1">
-        <v>1000</v>
+        <v>0.95</v>
       </c>
       <c r="P8" s="1">
+        <v>4000</v>
+      </c>
+      <c r="Q8" s="1">
+        <v>1000</v>
+      </c>
+      <c r="R8" s="1">
         <v>1</v>
       </c>
-      <c r="Q8" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="R8" s="1" t="s">
+      <c r="S8" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="T8" s="3" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="9" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A9" s="1">
         <v>8</v>
       </c>
@@ -990,46 +1057,52 @@
         <v>0.5</v>
       </c>
       <c r="F9" s="1">
-        <v>5</v>
+        <v>1000</v>
       </c>
       <c r="G9" s="1">
+        <v>5</v>
+      </c>
+      <c r="H9" s="1">
         <v>64</v>
       </c>
-      <c r="H9" s="1">
-        <v>2</v>
-      </c>
       <c r="I9" s="1">
+        <v>2</v>
+      </c>
+      <c r="J9" s="1">
         <v>0.2</v>
       </c>
-      <c r="J9" s="2">
-        <v>1E-3</v>
-      </c>
-      <c r="K9" s="1">
+      <c r="K9" s="2">
+        <v>2.9999999999999997E-4</v>
+      </c>
+      <c r="L9" s="2">
+        <v>1E-3</v>
+      </c>
+      <c r="M9" s="1">
         <v>0.01</v>
       </c>
-      <c r="L9" s="1">
+      <c r="N9" s="1">
         <v>0.99</v>
       </c>
-      <c r="M9" s="1">
-        <v>0.95</v>
-      </c>
-      <c r="N9" s="1">
-        <v>4000</v>
-      </c>
       <c r="O9" s="1">
+        <v>0.95</v>
+      </c>
+      <c r="P9" s="1">
+        <v>4000</v>
+      </c>
+      <c r="Q9" s="1">
         <v>200</v>
       </c>
-      <c r="P9" s="1">
-        <v>2</v>
-      </c>
-      <c r="Q9" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="R9" s="1" t="s">
+      <c r="R9" s="1">
+        <v>2</v>
+      </c>
+      <c r="S9" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="T9" s="3" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="10" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A10" s="1">
         <v>8</v>
       </c>
@@ -1046,46 +1119,52 @@
         <v>0.5</v>
       </c>
       <c r="F10" s="1">
-        <v>5</v>
+        <v>1000</v>
       </c>
       <c r="G10" s="1">
+        <v>5</v>
+      </c>
+      <c r="H10" s="1">
         <v>64</v>
       </c>
-      <c r="H10" s="1">
-        <v>2</v>
-      </c>
       <c r="I10" s="1">
+        <v>2</v>
+      </c>
+      <c r="J10" s="1">
         <v>0.2</v>
       </c>
-      <c r="J10" s="2">
-        <v>1E-3</v>
-      </c>
-      <c r="K10" s="1">
+      <c r="K10" s="2">
+        <v>2.9999999999999997E-4</v>
+      </c>
+      <c r="L10" s="2">
+        <v>1E-3</v>
+      </c>
+      <c r="M10" s="1">
         <v>0.01</v>
       </c>
-      <c r="L10" s="1">
+      <c r="N10" s="1">
         <v>0.99</v>
       </c>
-      <c r="M10" s="1">
-        <v>0.95</v>
-      </c>
-      <c r="N10" s="1">
-        <v>4000</v>
-      </c>
       <c r="O10" s="1">
+        <v>0.95</v>
+      </c>
+      <c r="P10" s="1">
+        <v>4000</v>
+      </c>
+      <c r="Q10" s="1">
         <v>200</v>
       </c>
-      <c r="P10" s="1">
-        <v>2</v>
-      </c>
-      <c r="Q10" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="R10" s="1" t="s">
+      <c r="R10" s="1">
+        <v>2</v>
+      </c>
+      <c r="S10" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="T10" s="3" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="11" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A11" s="1">
         <v>9</v>
       </c>
@@ -1102,46 +1181,52 @@
         <v>0.5</v>
       </c>
       <c r="F11" s="1">
-        <v>5</v>
+        <v>1000</v>
       </c>
       <c r="G11" s="1">
+        <v>5</v>
+      </c>
+      <c r="H11" s="1">
         <v>64</v>
       </c>
-      <c r="H11" s="1">
-        <v>2</v>
-      </c>
       <c r="I11" s="1">
+        <v>2</v>
+      </c>
+      <c r="J11" s="1">
         <v>0.2</v>
       </c>
-      <c r="J11" s="2">
-        <v>1E-3</v>
-      </c>
-      <c r="K11" s="1">
+      <c r="K11" s="2">
+        <v>2.9999999999999997E-4</v>
+      </c>
+      <c r="L11" s="2">
+        <v>1E-3</v>
+      </c>
+      <c r="M11" s="1">
         <v>0.01</v>
       </c>
-      <c r="L11" s="1">
+      <c r="N11" s="1">
         <v>0.99</v>
       </c>
-      <c r="M11" s="1">
-        <v>0.95</v>
-      </c>
-      <c r="N11" s="1">
-        <v>4000</v>
-      </c>
       <c r="O11" s="1">
+        <v>0.95</v>
+      </c>
+      <c r="P11" s="1">
+        <v>4000</v>
+      </c>
+      <c r="Q11" s="1">
         <v>200</v>
       </c>
-      <c r="P11" s="1">
-        <v>2</v>
-      </c>
-      <c r="Q11" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="R11" s="1" t="s">
+      <c r="R11" s="1">
+        <v>2</v>
+      </c>
+      <c r="S11" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="T11" s="3" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="12" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A12" s="1">
         <v>10</v>
       </c>
@@ -1158,46 +1243,52 @@
         <v>0.5</v>
       </c>
       <c r="F12" s="1">
-        <v>5</v>
+        <v>1000</v>
       </c>
       <c r="G12" s="1">
+        <v>5</v>
+      </c>
+      <c r="H12" s="1">
         <v>64</v>
       </c>
-      <c r="H12" s="1">
-        <v>2</v>
-      </c>
       <c r="I12" s="1">
+        <v>2</v>
+      </c>
+      <c r="J12" s="1">
         <v>0.2</v>
       </c>
-      <c r="J12" s="2">
-        <v>1E-3</v>
-      </c>
-      <c r="K12" s="1">
+      <c r="K12" s="2">
+        <v>2.9999999999999997E-4</v>
+      </c>
+      <c r="L12" s="2">
+        <v>1E-3</v>
+      </c>
+      <c r="M12" s="1">
         <v>0.01</v>
       </c>
-      <c r="L12" s="1">
+      <c r="N12" s="1">
         <v>0.99</v>
       </c>
-      <c r="M12" s="1">
-        <v>0.95</v>
-      </c>
-      <c r="N12" s="1">
-        <v>4000</v>
-      </c>
       <c r="O12" s="1">
+        <v>0.95</v>
+      </c>
+      <c r="P12" s="1">
+        <v>4000</v>
+      </c>
+      <c r="Q12" s="1">
         <v>200</v>
       </c>
-      <c r="P12" s="1">
-        <v>2</v>
-      </c>
-      <c r="Q12" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="R12" s="1" t="s">
+      <c r="R12" s="1">
+        <v>2</v>
+      </c>
+      <c r="S12" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="T12" s="3" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="13" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A13" s="1">
         <v>10</v>
       </c>
@@ -1214,46 +1305,52 @@
         <v>0.5</v>
       </c>
       <c r="F13" s="1">
-        <v>5</v>
+        <v>1000</v>
       </c>
       <c r="G13" s="1">
+        <v>5</v>
+      </c>
+      <c r="H13" s="1">
         <v>64</v>
       </c>
-      <c r="H13" s="1">
-        <v>2</v>
-      </c>
       <c r="I13" s="1">
+        <v>2</v>
+      </c>
+      <c r="J13" s="1">
         <v>0.2</v>
       </c>
-      <c r="J13" s="2">
-        <v>1E-3</v>
-      </c>
-      <c r="K13" s="1">
+      <c r="K13" s="2">
+        <v>2.9999999999999997E-4</v>
+      </c>
+      <c r="L13" s="2">
+        <v>1E-3</v>
+      </c>
+      <c r="M13" s="1">
         <v>0.01</v>
       </c>
-      <c r="L13" s="1">
+      <c r="N13" s="1">
         <v>0.99</v>
       </c>
-      <c r="M13" s="1">
-        <v>0.95</v>
-      </c>
-      <c r="N13" s="1">
-        <v>4000</v>
-      </c>
       <c r="O13" s="1">
+        <v>0.95</v>
+      </c>
+      <c r="P13" s="1">
+        <v>4000</v>
+      </c>
+      <c r="Q13" s="1">
         <v>200</v>
       </c>
-      <c r="P13" s="1">
-        <v>2</v>
-      </c>
-      <c r="Q13" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="R13" s="1" t="s">
+      <c r="R13" s="1">
+        <v>2</v>
+      </c>
+      <c r="S13" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="T13" s="3" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="14" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A14" s="1">
         <v>10</v>
       </c>
@@ -1270,46 +1367,52 @@
         <v>0.5</v>
       </c>
       <c r="F14" s="1">
-        <v>5</v>
+        <v>1000</v>
       </c>
       <c r="G14" s="1">
+        <v>5</v>
+      </c>
+      <c r="H14" s="1">
         <v>64</v>
       </c>
-      <c r="H14" s="1">
-        <v>2</v>
-      </c>
       <c r="I14" s="1">
+        <v>2</v>
+      </c>
+      <c r="J14" s="1">
         <v>0.2</v>
       </c>
-      <c r="J14" s="2">
-        <v>1E-3</v>
-      </c>
-      <c r="K14" s="1">
+      <c r="K14" s="2">
+        <v>2.9999999999999997E-4</v>
+      </c>
+      <c r="L14" s="2">
+        <v>1E-3</v>
+      </c>
+      <c r="M14" s="1">
         <v>0.01</v>
       </c>
-      <c r="L14" s="1">
+      <c r="N14" s="1">
         <v>0.99</v>
       </c>
-      <c r="M14" s="1">
-        <v>0.95</v>
-      </c>
-      <c r="N14" s="1">
-        <v>4000</v>
-      </c>
       <c r="O14" s="1">
+        <v>0.95</v>
+      </c>
+      <c r="P14" s="1">
+        <v>4000</v>
+      </c>
+      <c r="Q14" s="1">
         <v>200</v>
       </c>
-      <c r="P14" s="1">
-        <v>2</v>
-      </c>
-      <c r="Q14" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="R14" s="1" t="s">
+      <c r="R14" s="1">
+        <v>2</v>
+      </c>
+      <c r="S14" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="T14" s="3" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="15" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A15" s="1">
         <v>11</v>
       </c>
@@ -1326,46 +1429,52 @@
         <v>0.5</v>
       </c>
       <c r="F15" s="1">
-        <v>5</v>
+        <v>1000</v>
       </c>
       <c r="G15" s="1">
+        <v>5</v>
+      </c>
+      <c r="H15" s="1">
         <v>64</v>
       </c>
-      <c r="H15" s="1">
-        <v>2</v>
-      </c>
       <c r="I15" s="1">
+        <v>2</v>
+      </c>
+      <c r="J15" s="1">
         <v>0.2</v>
       </c>
-      <c r="J15" s="2">
-        <v>1E-3</v>
-      </c>
-      <c r="K15" s="1">
+      <c r="K15" s="2">
+        <v>2.9999999999999997E-4</v>
+      </c>
+      <c r="L15" s="2">
+        <v>1E-3</v>
+      </c>
+      <c r="M15" s="1">
         <v>0.01</v>
       </c>
-      <c r="L15" s="1">
+      <c r="N15" s="1">
         <v>0.99</v>
       </c>
-      <c r="M15" s="1">
-        <v>0.95</v>
-      </c>
-      <c r="N15" s="1">
-        <v>4000</v>
-      </c>
       <c r="O15" s="1">
+        <v>0.95</v>
+      </c>
+      <c r="P15" s="1">
+        <v>4000</v>
+      </c>
+      <c r="Q15" s="1">
         <v>200</v>
       </c>
-      <c r="P15" s="1">
+      <c r="R15" s="1">
         <v>3</v>
       </c>
-      <c r="Q15" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="R15" s="1" t="s">
+      <c r="S15" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="T15" s="3" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="16" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A16" s="1">
         <v>12</v>
       </c>
@@ -1382,46 +1491,52 @@
         <v>0.5</v>
       </c>
       <c r="F16" s="1">
-        <v>5</v>
+        <v>1000</v>
       </c>
       <c r="G16" s="1">
+        <v>5</v>
+      </c>
+      <c r="H16" s="1">
         <v>64</v>
       </c>
-      <c r="H16" s="1">
-        <v>2</v>
-      </c>
       <c r="I16" s="1">
+        <v>2</v>
+      </c>
+      <c r="J16" s="1">
         <v>0.2</v>
       </c>
-      <c r="J16" s="2">
-        <v>1E-3</v>
-      </c>
-      <c r="K16" s="1">
+      <c r="K16" s="2">
+        <v>2.9999999999999997E-4</v>
+      </c>
+      <c r="L16" s="2">
+        <v>1E-3</v>
+      </c>
+      <c r="M16" s="1">
         <v>0.01</v>
       </c>
-      <c r="L16" s="1">
+      <c r="N16" s="1">
         <v>0.99</v>
       </c>
-      <c r="M16" s="1">
-        <v>0.95</v>
-      </c>
-      <c r="N16" s="1">
-        <v>4000</v>
-      </c>
       <c r="O16" s="1">
+        <v>0.95</v>
+      </c>
+      <c r="P16" s="1">
+        <v>4000</v>
+      </c>
+      <c r="Q16" s="1">
         <v>200</v>
       </c>
-      <c r="P16" s="1">
-        <v>4</v>
-      </c>
-      <c r="Q16" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="R16" s="1" t="s">
+      <c r="R16" s="1">
+        <v>4</v>
+      </c>
+      <c r="S16" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="T16" s="3" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="17" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A17" s="1">
         <v>13</v>
       </c>
@@ -1438,46 +1553,52 @@
         <v>0.5</v>
       </c>
       <c r="F17" s="1">
-        <v>5</v>
+        <v>1000</v>
       </c>
       <c r="G17" s="1">
+        <v>5</v>
+      </c>
+      <c r="H17" s="1">
         <v>128</v>
       </c>
-      <c r="H17" s="1">
-        <v>2</v>
-      </c>
       <c r="I17" s="1">
+        <v>2</v>
+      </c>
+      <c r="J17" s="1">
         <v>0.2</v>
       </c>
-      <c r="J17" s="2">
-        <v>1E-3</v>
-      </c>
-      <c r="K17" s="1">
+      <c r="K17" s="2">
+        <v>2.9999999999999997E-4</v>
+      </c>
+      <c r="L17" s="2">
+        <v>1E-3</v>
+      </c>
+      <c r="M17" s="1">
         <v>0.01</v>
       </c>
-      <c r="L17" s="1">
+      <c r="N17" s="1">
         <v>0.99</v>
       </c>
-      <c r="M17" s="1">
-        <v>0.95</v>
-      </c>
-      <c r="N17" s="1">
-        <v>4000</v>
-      </c>
       <c r="O17" s="1">
+        <v>0.95</v>
+      </c>
+      <c r="P17" s="1">
+        <v>4000</v>
+      </c>
+      <c r="Q17" s="1">
         <v>200</v>
       </c>
-      <c r="P17" s="1">
-        <v>2</v>
-      </c>
-      <c r="Q17" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="R17" s="1" t="s">
+      <c r="R17" s="1">
+        <v>2</v>
+      </c>
+      <c r="S17" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="T17" s="3" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="18" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A18" s="1">
         <v>14</v>
       </c>
@@ -1494,46 +1615,52 @@
         <v>0.5</v>
       </c>
       <c r="F18" s="1">
-        <v>5</v>
+        <v>1000</v>
       </c>
       <c r="G18" s="1">
+        <v>5</v>
+      </c>
+      <c r="H18" s="1">
         <v>128</v>
       </c>
-      <c r="H18" s="1">
-        <v>2</v>
-      </c>
       <c r="I18" s="1">
+        <v>2</v>
+      </c>
+      <c r="J18" s="1">
         <v>0.1</v>
       </c>
-      <c r="J18" s="2">
-        <v>1E-3</v>
-      </c>
-      <c r="K18" s="1">
+      <c r="K18" s="2">
+        <v>2.9999999999999997E-4</v>
+      </c>
+      <c r="L18" s="2">
+        <v>1E-3</v>
+      </c>
+      <c r="M18" s="1">
         <v>0.01</v>
       </c>
-      <c r="L18" s="1">
+      <c r="N18" s="1">
         <v>0.99</v>
       </c>
-      <c r="M18" s="1">
-        <v>0.95</v>
-      </c>
-      <c r="N18" s="1">
-        <v>4000</v>
-      </c>
       <c r="O18" s="1">
+        <v>0.95</v>
+      </c>
+      <c r="P18" s="1">
+        <v>4000</v>
+      </c>
+      <c r="Q18" s="1">
         <v>200</v>
       </c>
-      <c r="P18" s="1">
-        <v>2</v>
-      </c>
-      <c r="Q18" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="R18" s="1" t="s">
+      <c r="R18" s="1">
+        <v>2</v>
+      </c>
+      <c r="S18" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="T18" s="3" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="19" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A19" s="1">
         <v>15</v>
       </c>
@@ -1550,46 +1677,52 @@
         <v>0.5</v>
       </c>
       <c r="F19" s="1">
-        <v>5</v>
+        <v>1000</v>
       </c>
       <c r="G19" s="1">
+        <v>5</v>
+      </c>
+      <c r="H19" s="1">
         <v>128</v>
       </c>
-      <c r="H19" s="1">
-        <v>2</v>
-      </c>
       <c r="I19" s="1">
+        <v>2</v>
+      </c>
+      <c r="J19" s="1">
         <v>0.1</v>
       </c>
-      <c r="J19" s="2">
-        <v>1E-3</v>
-      </c>
-      <c r="K19" s="1">
+      <c r="K19" s="2">
+        <v>2.9999999999999997E-4</v>
+      </c>
+      <c r="L19" s="2">
+        <v>1E-3</v>
+      </c>
+      <c r="M19" s="1">
         <v>1.4999999999999999E-2</v>
       </c>
-      <c r="L19" s="1">
+      <c r="N19" s="1">
         <v>0.99</v>
       </c>
-      <c r="M19" s="1">
-        <v>0.95</v>
-      </c>
-      <c r="N19" s="1">
-        <v>4000</v>
-      </c>
       <c r="O19" s="1">
+        <v>0.95</v>
+      </c>
+      <c r="P19" s="1">
+        <v>4000</v>
+      </c>
+      <c r="Q19" s="1">
         <v>200</v>
       </c>
-      <c r="P19" s="1">
-        <v>2</v>
-      </c>
-      <c r="Q19" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="R19" s="1" t="s">
+      <c r="R19" s="1">
+        <v>2</v>
+      </c>
+      <c r="S19" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="T19" s="3" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="20" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A20" s="1">
         <v>15</v>
       </c>
@@ -1606,46 +1739,52 @@
         <v>0.5</v>
       </c>
       <c r="F20" s="1">
-        <v>5</v>
+        <v>1000</v>
       </c>
       <c r="G20" s="1">
+        <v>5</v>
+      </c>
+      <c r="H20" s="1">
         <v>128</v>
       </c>
-      <c r="H20" s="1">
-        <v>2</v>
-      </c>
       <c r="I20" s="1">
+        <v>2</v>
+      </c>
+      <c r="J20" s="1">
         <v>0.1</v>
       </c>
-      <c r="J20" s="2">
-        <v>1E-3</v>
-      </c>
-      <c r="K20" s="1">
+      <c r="K20" s="2">
+        <v>2.9999999999999997E-4</v>
+      </c>
+      <c r="L20" s="2">
+        <v>1E-3</v>
+      </c>
+      <c r="M20" s="1">
         <v>1.4999999999999999E-2</v>
       </c>
-      <c r="L20" s="1">
+      <c r="N20" s="1">
         <v>0.99</v>
       </c>
-      <c r="M20" s="1">
-        <v>0.95</v>
-      </c>
-      <c r="N20" s="1">
-        <v>4000</v>
-      </c>
       <c r="O20" s="1">
+        <v>0.95</v>
+      </c>
+      <c r="P20" s="1">
+        <v>4000</v>
+      </c>
+      <c r="Q20" s="1">
         <v>800</v>
       </c>
-      <c r="P20" s="1">
-        <v>2</v>
-      </c>
-      <c r="Q20" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="R20" s="1" t="s">
+      <c r="R20" s="1">
+        <v>2</v>
+      </c>
+      <c r="S20" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="T20" s="3" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="21" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A21" s="1">
         <v>16</v>
       </c>
@@ -1662,44 +1801,178 @@
         <v>0.5</v>
       </c>
       <c r="F21" s="1">
-        <v>5</v>
+        <v>1000</v>
       </c>
       <c r="G21" s="1">
+        <v>5</v>
+      </c>
+      <c r="H21" s="1">
         <v>128</v>
       </c>
-      <c r="H21" s="1">
-        <v>2</v>
-      </c>
       <c r="I21" s="1">
+        <v>2</v>
+      </c>
+      <c r="J21" s="1">
         <v>0.1</v>
       </c>
-      <c r="J21" s="2">
+      <c r="K21" s="2">
+        <v>2.9999999999999997E-4</v>
+      </c>
+      <c r="L21" s="2">
         <v>5.0000000000000001E-4</v>
       </c>
-      <c r="K21" s="1">
+      <c r="M21" s="1">
         <v>1.4999999999999999E-2</v>
       </c>
-      <c r="L21" s="1">
+      <c r="N21" s="1">
         <v>0.99</v>
       </c>
-      <c r="M21" s="1">
-        <v>0.95</v>
-      </c>
-      <c r="N21" s="1">
-        <v>4000</v>
-      </c>
       <c r="O21" s="1">
-        <v>1000</v>
+        <v>0.95</v>
       </c>
       <c r="P21" s="1">
-        <v>2</v>
-      </c>
-      <c r="Q21" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="R21" s="1" t="s">
+        <v>4000</v>
+      </c>
+      <c r="Q21" s="1">
+        <v>1000</v>
+      </c>
+      <c r="R21" s="1">
+        <v>2</v>
+      </c>
+      <c r="S21" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="T21" s="3" t="s">
         <v>30</v>
       </c>
+    </row>
+    <row r="22" spans="1:20" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A22" s="1">
+        <v>17</v>
+      </c>
+      <c r="B22" s="1">
+        <v>2</v>
+      </c>
+      <c r="C22" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="D22" s="1">
+        <v>4</v>
+      </c>
+      <c r="E22" s="1">
+        <v>0.5</v>
+      </c>
+      <c r="F22" s="1">
+        <v>2000</v>
+      </c>
+      <c r="G22" s="1">
+        <v>5</v>
+      </c>
+      <c r="H22" s="1">
+        <v>128</v>
+      </c>
+      <c r="I22" s="1">
+        <v>2</v>
+      </c>
+      <c r="J22" s="1">
+        <v>0.1</v>
+      </c>
+      <c r="K22" s="2">
+        <v>1E-4</v>
+      </c>
+      <c r="L22" s="2">
+        <v>1E-3</v>
+      </c>
+      <c r="M22" s="1">
+        <v>0.01</v>
+      </c>
+      <c r="N22" s="1">
+        <v>0.99</v>
+      </c>
+      <c r="O22" s="1">
+        <v>0.95</v>
+      </c>
+      <c r="P22" s="1">
+        <v>4000</v>
+      </c>
+      <c r="Q22" s="1">
+        <v>200</v>
+      </c>
+      <c r="R22" s="1">
+        <v>2</v>
+      </c>
+      <c r="S22" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="T22" s="3" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="23" spans="1:20" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A23" s="1">
+        <v>17</v>
+      </c>
+      <c r="B23" s="1">
+        <v>2</v>
+      </c>
+      <c r="C23" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="D23" s="1">
+        <v>4</v>
+      </c>
+      <c r="E23" s="1">
+        <v>0.5</v>
+      </c>
+      <c r="F23" s="1">
+        <v>2000</v>
+      </c>
+      <c r="G23" s="1">
+        <v>5</v>
+      </c>
+      <c r="H23" s="1">
+        <v>128</v>
+      </c>
+      <c r="I23" s="1">
+        <v>2</v>
+      </c>
+      <c r="J23" s="1">
+        <v>0.1</v>
+      </c>
+      <c r="K23" s="2">
+        <v>1E-4</v>
+      </c>
+      <c r="L23" s="2">
+        <v>1E-3</v>
+      </c>
+      <c r="M23" s="1">
+        <v>0.01</v>
+      </c>
+      <c r="N23" s="1">
+        <v>0.99</v>
+      </c>
+      <c r="O23" s="1">
+        <v>0.95</v>
+      </c>
+      <c r="P23" s="1">
+        <v>4000</v>
+      </c>
+      <c r="Q23" s="1">
+        <v>200</v>
+      </c>
+      <c r="R23" s="1">
+        <v>2</v>
+      </c>
+      <c r="S23" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="T23" s="3" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="24" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="K24" s="2"/>
+      <c r="L24" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
updated folder structure and updated documentation
</commit_message>
<xml_diff>
--- a/documentation/trials.xlsx
+++ b/documentation/trials.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ocean\Documents\GitHub\CPTS-437-DDPG-RSSI-Car\documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BA3D0B27-FDF7-407E-BFAE-6A6DD6E9B94B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{37F7D4FE-3A98-4266-BC74-2C2D23914B94}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{496E26A4-E262-4A0D-A9DD-90AD4307AC27}"/>
   </bookViews>
@@ -526,8 +526,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DD51C088-492E-456A-BAA7-804EE5452A68}">
   <dimension ref="A1:T24"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A11" workbookViewId="0">
-      <selection activeCell="E24" sqref="E24"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>